<commit_message>
error handling and guide left
</commit_message>
<xml_diff>
--- a/Process-RR-Mapping/Process-RR-Mapping.xlsx
+++ b/Process-RR-Mapping/Process-RR-Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\BluePrism-Automated-Testing\Process-RR-Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F6BBFD-E9BC-4F9C-A799-BDCE82465324}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82285269-1049-46B9-9EDA-DB55B2209D07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Sequence</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Test Results Data File location</t>
+  </si>
+  <si>
+    <t>New release file name</t>
+  </si>
+  <si>
+    <t>Release file location</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>C:\Users\AEasow\PycharmProjects\TestCoverage\release\Registration Process.bprelease</t>
+  </si>
+  <si>
+    <t>testcoverage.bprelease</t>
   </si>
 </sst>
 </file>
@@ -122,7 +137,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,17 +160,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,9 +481,11 @@
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="78.28515625" customWidth="1"/>
     <col min="10" max="10" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -487,8 +516,14 @@
       <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -515,10 +550,16 @@
         <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -547,8 +588,10 @@
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -577,8 +620,10 @@
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -589,8 +634,10 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -601,8 +648,10 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -613,8 +662,10 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -625,8 +676,10 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -637,8 +690,10 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -649,8 +704,10 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -661,8 +718,10 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -673,8 +732,10 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -685,8 +746,10 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -697,8 +760,10 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -709,8 +774,10 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -721,8 +788,10 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -733,8 +802,10 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -745,8 +816,10 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -757,8 +830,10 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -769,8 +844,10 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -781,8 +858,10 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -793,8 +872,10 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -805,8 +886,10 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -817,8 +900,10 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -829,8 +914,10 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -841,8 +928,10 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -853,8 +942,10 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -865,8 +956,10 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -877,8 +970,10 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -889,8 +984,10 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -901,6 +998,8 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed data not required
</commit_message>
<xml_diff>
--- a/Process-RR-Mapping/Process-RR-Mapping.xlsx
+++ b/Process-RR-Mapping/Process-RR-Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\BluePrism-Automated-Testing\Process-RR-Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82285269-1049-46B9-9EDA-DB55B2209D07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1BD65C-C516-49E5-B64B-9E4A3065B2BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Sequence</t>
   </si>
@@ -45,12 +45,6 @@
     <t>BP0300</t>
   </si>
   <si>
-    <t>Test APAC</t>
-  </si>
-  <si>
-    <t>First Process</t>
-  </si>
-  <si>
     <t>SSO Flag</t>
   </si>
   <si>
@@ -76,12 +70,6 @@
   </si>
   <si>
     <t>C:\GIT\BluePrism-Automated-Testing\Test Results\Submit Regstration Process.xlsx</t>
-  </si>
-  <si>
-    <t>C:\GIT\BluePrism-Automated-Testing\Test Results\Test APAC.xlsx</t>
-  </si>
-  <si>
-    <t>C:\GIT\BluePrism-Automated-Testing\Test Results\First Process.xlsx</t>
   </si>
   <si>
     <t>Test Results Data File location</t>
@@ -463,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,28 +487,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -537,89 +525,53 @@
         <v>8182</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8183</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8181</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
@@ -973,34 +925,6 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>